<commit_message>
First Complete Successful Commit.
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
+++ b/DataDrivenFramework/src/test/resources/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smanem/GitHub/SeleniumDataDrivenFramework/DataDrivenFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE64D379-9CD5-E74D-BB19-64A26D682899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17200" windowHeight="5380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -103,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,16 +415,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -431,7 +432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -439,7 +440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -447,7 +448,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -461,16 +462,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,7 +488,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -504,7 +505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -521,7 +522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -535,10 +536,10 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -552,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -561,16 +562,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>

</xml_diff>